<commit_message>
added new test cases for setting tabs
</commit_message>
<xml_diff>
--- a/Excel/Test.xlsx
+++ b/Excel/Test.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7480" windowHeight="4970"/>
   </bookViews>
   <sheets>
-    <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="ATC_CDV" sheetId="1" r:id="rId1"/>
+    <sheet name="Articles" sheetId="2" r:id="rId2"/>
+    <sheet name="supplier_appro" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,42 +21,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>S4333164</t>
-  </si>
-  <si>
-    <t>sg!t@2020</t>
-  </si>
-  <si>
-    <t>s433</t>
-  </si>
-  <si>
-    <t>S212</t>
-  </si>
-  <si>
-    <t>P8099488</t>
-  </si>
-  <si>
-    <t>P@ssword@2020</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+  <si>
+    <t>TEST MANAGER 1</t>
+  </si>
+  <si>
+    <t>H9</t>
+  </si>
+  <si>
+    <t>TEST SELLER 1</t>
+  </si>
+  <si>
+    <t>TEST MANAGER 2</t>
+  </si>
+  <si>
+    <t>TEST SELLER 2</t>
+  </si>
+  <si>
+    <t>TEST MANAGER 3</t>
+  </si>
+  <si>
+    <t>TEST SELLER 3</t>
+  </si>
+  <si>
+    <t>TEST MANAGER 4</t>
+  </si>
+  <si>
+    <t>TEST SELLER 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -68,7 +71,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -76,38 +79,20 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -386,46 +371,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="17.36328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>2201</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="D1">
+        <v>300</v>
+      </c>
+      <c r="E1">
+        <v>3301</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2202</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>300</v>
+      </c>
+      <c r="E2">
+        <v>3302</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2203</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>300</v>
+      </c>
+      <c r="E3">
+        <v>3303</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2204</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>300</v>
+      </c>
+      <c r="E4">
+        <v>3304</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new test cases on manage setting menu
</commit_message>
<xml_diff>
--- a/Excel/Test.xlsx
+++ b/Excel/Test.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7480" windowHeight="4970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14050" windowHeight="3450" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ATC_CDV" sheetId="1" r:id="rId1"/>
     <sheet name="Articles" sheetId="2" r:id="rId2"/>
     <sheet name="supplier_appro" sheetId="3" r:id="rId3"/>
+    <sheet name="supplier_producer" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:N10"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>TEST MANAGER 1</t>
   </si>
@@ -48,6 +50,63 @@
   </si>
   <si>
     <t>TEST SELLER 4</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>A3861</t>
+  </si>
+  <si>
+    <t>B2041</t>
+  </si>
+  <si>
+    <t>B2316</t>
+  </si>
+  <si>
+    <t>B6185</t>
+  </si>
+  <si>
+    <t>B6340</t>
+  </si>
+  <si>
+    <t>B0176</t>
+  </si>
+  <si>
+    <t>B1392</t>
+  </si>
+  <si>
+    <t>B0553</t>
+  </si>
+  <si>
+    <t>06687</t>
+  </si>
+  <si>
+    <t>06686</t>
+  </si>
+  <si>
+    <t>06685</t>
+  </si>
+  <si>
+    <t>06684</t>
+  </si>
+  <si>
+    <t>06683</t>
+  </si>
+  <si>
+    <t>06682</t>
+  </si>
+  <si>
+    <t>06681</t>
+  </si>
+  <si>
+    <t>06680</t>
+  </si>
+  <si>
+    <t>06679</t>
   </si>
 </sst>
 </file>
@@ -83,12 +142,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -373,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -472,26 +534,202 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="2">
+        <v>6509975</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>6527018</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>6527118</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>6528319</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>6522478</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>6522578</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>6524481</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>6511396</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>6512197</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>